<commit_message>
add 2 decimal to moy
</commit_message>
<xml_diff>
--- a/RICATTE_SUBLET.xlsx
+++ b/RICATTE_SUBLET.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Clement\IUT\S2\IHM\Lazarus work\GestionScolaire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C2C0C4A-8E4D-4F26-8785-4A5B9A579BDD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{403BD5AC-598C-4DDD-A64B-B7090FF1AB8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1301,351 +1301,21 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="195">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="162">
     <dxf>
       <font>
         <color theme="0"/>
@@ -3803,8 +3473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F111"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A81" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E102" sqref="E102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -3822,12 +3492,12 @@
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:6" s="1" customFormat="1" ht="67.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
       <c r="E3" s="25"/>
     </row>
     <row r="4" spans="1:6" s="1" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3945,7 +3615,7 @@
         <v>28</v>
       </c>
       <c r="D17" s="3"/>
-      <c r="E17" s="41" t="s">
+      <c r="E17" s="39" t="s">
         <v>48</v>
       </c>
     </row>
@@ -3965,7 +3635,7 @@
         <v>29</v>
       </c>
       <c r="D19" s="5"/>
-      <c r="E19" s="41" t="s">
+      <c r="E19" s="39" t="s">
         <v>48</v>
       </c>
     </row>
@@ -3976,7 +3646,7 @@
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
-      <c r="E20" s="41" t="s">
+      <c r="E20" s="39" t="s">
         <v>48</v>
       </c>
     </row>
@@ -3987,7 +3657,7 @@
         <v>4</v>
       </c>
       <c r="D21" s="3"/>
-      <c r="E21" s="41" t="s">
+      <c r="E21" s="39" t="s">
         <v>48</v>
       </c>
     </row>
@@ -4721,11 +4391,11 @@
     </row>
     <row r="92" spans="1:5" ht="76.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
-      <c r="B92" s="39" t="s">
+      <c r="B92" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="C92" s="39"/>
-      <c r="D92" s="39"/>
+      <c r="C92" s="40"/>
+      <c r="D92" s="40"/>
       <c r="E92" s="27"/>
     </row>
     <row r="93" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -4818,7 +4488,7 @@
       </c>
       <c r="D101" s="3"/>
       <c r="E101" s="26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -4829,7 +4499,7 @@
       </c>
       <c r="D102" s="3"/>
       <c r="E102" s="26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -4923,563 +4593,563 @@
     <mergeCell ref="A3:D3"/>
   </mergeCells>
   <conditionalFormatting sqref="E11 E108 E106">
-    <cfRule type="cellIs" dxfId="194" priority="187" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="193" priority="188" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="161" priority="187" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="160" priority="188" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E11)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="192" priority="189">
+    <cfRule type="expression" dxfId="159" priority="189">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="191" priority="184" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="190" priority="185" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="158" priority="184" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="157" priority="185" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E12)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="189" priority="186">
+    <cfRule type="expression" dxfId="156" priority="186">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="cellIs" dxfId="188" priority="181" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="187" priority="182" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="155" priority="181" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="154" priority="182" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E13)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="186" priority="183">
+    <cfRule type="expression" dxfId="153" priority="183">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="cellIs" dxfId="185" priority="178" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="184" priority="179" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="152" priority="178" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="151" priority="179" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E15)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="183" priority="180">
+    <cfRule type="expression" dxfId="150" priority="180">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="176" priority="169" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="175" priority="170" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="149" priority="169" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="148" priority="170" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E23)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="174" priority="171">
+    <cfRule type="expression" dxfId="147" priority="171">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26">
-    <cfRule type="cellIs" dxfId="173" priority="166" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="172" priority="167" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="146" priority="166" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="145" priority="167" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E26)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="171" priority="168">
+    <cfRule type="expression" dxfId="144" priority="168">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E33 E41:E43">
-    <cfRule type="cellIs" dxfId="170" priority="163" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="169" priority="164" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="143" priority="163" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="142" priority="164" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E33)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="168" priority="165">
+    <cfRule type="expression" dxfId="141" priority="165">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E46">
-    <cfRule type="cellIs" dxfId="167" priority="160" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="166" priority="161" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="140" priority="160" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="139" priority="161" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E46)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="165" priority="162">
+    <cfRule type="expression" dxfId="138" priority="162">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E49:E56">
-    <cfRule type="cellIs" dxfId="95" priority="157" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="158" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="137" priority="157" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="136" priority="158" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E49)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="93" priority="159">
+    <cfRule type="expression" dxfId="135" priority="159">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E78">
-    <cfRule type="cellIs" dxfId="155" priority="145" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="154" priority="146" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="134" priority="145" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="133" priority="146" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E78)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="153" priority="147">
+    <cfRule type="expression" dxfId="132" priority="147">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E97:E98">
-    <cfRule type="cellIs" dxfId="143" priority="133" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="142" priority="134" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="131" priority="133" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="130" priority="134" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E97)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="141" priority="135">
+    <cfRule type="expression" dxfId="129" priority="135">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E101:E102">
-    <cfRule type="cellIs" dxfId="140" priority="130" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="139" priority="131" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="128" priority="130" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="127" priority="131" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E101)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="138" priority="132">
+    <cfRule type="expression" dxfId="126" priority="132">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E111">
-    <cfRule type="cellIs" dxfId="137" priority="124" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="136" priority="125" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="125" priority="124" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="124" priority="125" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E111)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="135" priority="126">
+    <cfRule type="expression" dxfId="123" priority="126">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E27">
-    <cfRule type="cellIs" dxfId="134" priority="121" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="133" priority="122" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="122" priority="121" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="121" priority="122" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E27)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="132" priority="123">
+    <cfRule type="expression" dxfId="120" priority="123">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E28">
-    <cfRule type="cellIs" dxfId="131" priority="118" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="130" priority="119" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="119" priority="118" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="118" priority="119" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E28)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="129" priority="120">
+    <cfRule type="expression" dxfId="117" priority="120">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29">
-    <cfRule type="cellIs" dxfId="128" priority="115" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="127" priority="116" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="116" priority="115" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="115" priority="116" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E29)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="126" priority="117">
+    <cfRule type="expression" dxfId="114" priority="117">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30">
-    <cfRule type="cellIs" dxfId="125" priority="112" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="124" priority="113" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="113" priority="112" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="112" priority="113" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E30)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="123" priority="114">
+    <cfRule type="expression" dxfId="111" priority="114">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31">
-    <cfRule type="cellIs" dxfId="122" priority="109" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="121" priority="110" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="110" priority="109" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="109" priority="110" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E31)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="120" priority="111">
+    <cfRule type="expression" dxfId="108" priority="111">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34">
-    <cfRule type="cellIs" dxfId="119" priority="106" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="118" priority="107" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="107" priority="106" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="106" priority="107" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E34)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="117" priority="108">
+    <cfRule type="expression" dxfId="105" priority="108">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35">
-    <cfRule type="cellIs" dxfId="116" priority="103" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="115" priority="104" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="104" priority="103" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="103" priority="104" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E35)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="114" priority="105">
+    <cfRule type="expression" dxfId="102" priority="105">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36">
-    <cfRule type="cellIs" dxfId="113" priority="100" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="112" priority="101" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="101" priority="100" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="100" priority="101" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E36)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="111" priority="102">
+    <cfRule type="expression" dxfId="99" priority="102">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E37">
-    <cfRule type="cellIs" dxfId="110" priority="97" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="109" priority="98" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="98" priority="97" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="97" priority="98" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E37)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="108" priority="99">
+    <cfRule type="expression" dxfId="96" priority="99">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E38">
-    <cfRule type="cellIs" dxfId="107" priority="94" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="106" priority="95" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="95" priority="94" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="94" priority="95" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E38)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="105" priority="96">
+    <cfRule type="expression" dxfId="93" priority="96">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E39">
-    <cfRule type="cellIs" dxfId="104" priority="91" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="103" priority="92" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="92" priority="91" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="91" priority="92" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E39)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="93">
+    <cfRule type="expression" dxfId="90" priority="93">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E40">
-    <cfRule type="cellIs" dxfId="101" priority="88" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="100" priority="89" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="89" priority="88" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="88" priority="89" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E40)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="99" priority="90">
+    <cfRule type="expression" dxfId="87" priority="90">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E58">
-    <cfRule type="cellIs" dxfId="92" priority="85" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="86" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="86" priority="85" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="85" priority="86" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E58)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="90" priority="87">
+    <cfRule type="expression" dxfId="84" priority="87">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E59">
-    <cfRule type="cellIs" dxfId="89" priority="82" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="83" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="83" priority="82" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="82" priority="83" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E59)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="87" priority="84">
+    <cfRule type="expression" dxfId="81" priority="84">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E60">
-    <cfRule type="cellIs" dxfId="86" priority="79" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="80" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="80" priority="79" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="79" priority="80" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E60)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="84" priority="81">
+    <cfRule type="expression" dxfId="78" priority="81">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E61">
-    <cfRule type="cellIs" dxfId="83" priority="76" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="77" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="77" priority="76" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="76" priority="77" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E61)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="78">
+    <cfRule type="expression" dxfId="75" priority="78">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E62">
-    <cfRule type="cellIs" dxfId="80" priority="73" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="74" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="74" priority="73" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="73" priority="74" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E62)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="75">
+    <cfRule type="expression" dxfId="72" priority="75">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E63">
-    <cfRule type="cellIs" dxfId="77" priority="70" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="71" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="71" priority="70" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="70" priority="71" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E63)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="72">
+    <cfRule type="expression" dxfId="69" priority="72">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E64">
-    <cfRule type="cellIs" dxfId="74" priority="67" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="68" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="68" priority="67" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="67" priority="68" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E64)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="69">
+    <cfRule type="expression" dxfId="66" priority="69">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E65">
-    <cfRule type="cellIs" dxfId="71" priority="64" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="65" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="65" priority="64" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="64" priority="65" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E65)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="66">
+    <cfRule type="expression" dxfId="63" priority="66">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E66">
-    <cfRule type="cellIs" dxfId="68" priority="61" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="62" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="62" priority="61" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="61" priority="62" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E66)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="63">
+    <cfRule type="expression" dxfId="60" priority="63">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E67">
-    <cfRule type="cellIs" dxfId="65" priority="58" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="59" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="59" priority="58" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="58" priority="59" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E67)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="60">
+    <cfRule type="expression" dxfId="57" priority="60">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E70">
-    <cfRule type="cellIs" dxfId="62" priority="55" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="56" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="56" priority="55" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="55" priority="56" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E70)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="57">
+    <cfRule type="expression" dxfId="54" priority="57">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E71">
-    <cfRule type="cellIs" dxfId="59" priority="52" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="53" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="53" priority="52" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="52" priority="53" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E71)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="54">
+    <cfRule type="expression" dxfId="51" priority="54">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E72">
-    <cfRule type="cellIs" dxfId="56" priority="49" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="50" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="50" priority="49" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="49" priority="50" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E72)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="51">
+    <cfRule type="expression" dxfId="48" priority="51">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E75">
-    <cfRule type="cellIs" dxfId="53" priority="46" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="47" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="47" priority="46" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="46" priority="47" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E75)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="48">
+    <cfRule type="expression" dxfId="45" priority="48">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E76">
-    <cfRule type="cellIs" dxfId="50" priority="43" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="44" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="44" priority="43" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="43" priority="44" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E76)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="45">
+    <cfRule type="expression" dxfId="42" priority="45">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E80">
-    <cfRule type="cellIs" dxfId="47" priority="40" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="41" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="41" priority="40" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="40" priority="41" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E80)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="42">
+    <cfRule type="expression" dxfId="39" priority="42">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E82">
-    <cfRule type="cellIs" dxfId="44" priority="37" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="38" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="38" priority="37" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="37" priority="38" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E82)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="39">
+    <cfRule type="expression" dxfId="36" priority="39">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E83">
-    <cfRule type="cellIs" dxfId="41" priority="34" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="35" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="35" priority="34" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="34" priority="35" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E83)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="36">
+    <cfRule type="expression" dxfId="33" priority="36">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E84">
-    <cfRule type="cellIs" dxfId="38" priority="31" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="32" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="32" priority="31" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="31" priority="32" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E84)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="33">
+    <cfRule type="expression" dxfId="30" priority="33">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E85">
-    <cfRule type="cellIs" dxfId="35" priority="28" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="29" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="29" priority="28" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="28" priority="29" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E85)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="30">
+    <cfRule type="expression" dxfId="27" priority="30">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E86">
-    <cfRule type="cellIs" dxfId="32" priority="25" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="26" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="26" priority="25" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="25" priority="26" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E86)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="27">
+    <cfRule type="expression" dxfId="24" priority="27">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E87">
-    <cfRule type="cellIs" dxfId="29" priority="22" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="23" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="23" priority="22" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E87)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="24">
+    <cfRule type="expression" dxfId="21" priority="24">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E88">
-    <cfRule type="cellIs" dxfId="26" priority="19" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="20" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="20" priority="19" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E88)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="21">
+    <cfRule type="expression" dxfId="18" priority="21">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E89">
-    <cfRule type="cellIs" dxfId="23" priority="16" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="17" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E89)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="18">
+    <cfRule type="expression" dxfId="15" priority="18">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E90">
-    <cfRule type="cellIs" dxfId="20" priority="13" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="14" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E90)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="15">
+    <cfRule type="expression" dxfId="12" priority="15">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E91">
-    <cfRule type="cellIs" dxfId="17" priority="10" operator="equal">
-      <formula>"NON"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="11" operator="containsText" text="OUI">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+      <formula>"NON"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="OUI">
       <formula>NOT(ISERROR(SEARCH("OUI",E91)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="12">
+    <cfRule type="expression" dxfId="9" priority="12">
       <formula>$E$7</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>